<commit_message>
Atualiza dashboard conforme reunião Amanda
</commit_message>
<xml_diff>
--- a/Base de Processos VLF.xlsx
+++ b/Base de Processos VLF.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://vlfadv-my.sharepoint.com/personal/henrique_abrantes_vlf_adv_br/Documents/Área de Trabalho/Projetos VLF/apresentacao_inter/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="42" documentId="8_{55415661-EC0E-4DC1-A797-3BD06E012560}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D96876B6-E43F-4FBC-AC1E-DAB3A79D9EBA}"/>
+  <xr:revisionPtr revIDLastSave="43" documentId="8_{55415661-EC0E-4DC1-A797-3BD06E012560}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{32EED1F6-A6DE-47E2-A63E-99D86B2C877D}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -6705,11 +6705,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:AP1048576"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A192" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H398" sqref="H398"/>
+    <sheetView tabSelected="1" topLeftCell="T1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A397" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="Z2" sqref="Z2:Z397"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7396,7 +7397,7 @@
         <v>1479</v>
       </c>
     </row>
-    <row r="6" spans="1:42" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:42" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>27</v>
       </c>
@@ -8124,7 +8125,7 @@
         <v>1479</v>
       </c>
     </row>
-    <row r="12" spans="1:42" ht="285" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:42" ht="285" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" s="17" t="s">
         <v>33</v>
       </c>
@@ -8634,7 +8635,7 @@
         <v>1479</v>
       </c>
     </row>
-    <row r="16" spans="1:42" ht="45" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:42" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
         <v>37</v>
       </c>
@@ -9492,7 +9493,7 @@
         <v>1479</v>
       </c>
     </row>
-    <row r="23" spans="1:42" ht="60" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:42" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" s="17" t="s">
         <v>43</v>
       </c>
@@ -11036,7 +11037,7 @@
         <v>1479</v>
       </c>
     </row>
-    <row r="35" spans="1:42" ht="75" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:42" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" s="17" t="s">
         <v>55</v>
       </c>
@@ -12832,7 +12833,7 @@
         <v>1479</v>
       </c>
     </row>
-    <row r="49" spans="1:42" ht="45" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:42" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49" s="17" t="s">
         <v>69</v>
       </c>
@@ -15908,7 +15909,7 @@
         <v>1479</v>
       </c>
     </row>
-    <row r="73" spans="1:42" ht="30" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:42" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A73" s="17" t="s">
         <v>93</v>
       </c>
@@ -16932,7 +16933,7 @@
         <v>1479</v>
       </c>
     </row>
-    <row r="81" spans="1:42" ht="60" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:42" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A81" s="17" t="s">
         <v>101</v>
       </c>
@@ -18078,7 +18079,7 @@
         <v>1479</v>
       </c>
     </row>
-    <row r="90" spans="1:42" ht="45" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:42" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A90" s="17" t="s">
         <v>110</v>
       </c>
@@ -20113,7 +20114,7 @@
         <v>1479</v>
       </c>
     </row>
-    <row r="106" spans="1:42" ht="60" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:42" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A106" s="17" t="s">
         <v>126</v>
       </c>
@@ -20369,7 +20370,7 @@
         <v>1479</v>
       </c>
     </row>
-    <row r="108" spans="1:42" ht="75" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:42" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A108" s="17" t="s">
         <v>128</v>
       </c>
@@ -21265,7 +21266,7 @@
         <v>1479</v>
       </c>
     </row>
-    <row r="115" spans="1:42" ht="150" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:42" ht="150" hidden="1" x14ac:dyDescent="0.25">
       <c r="A115" s="17" t="s">
         <v>135</v>
       </c>
@@ -21511,7 +21512,7 @@
         <v>1479</v>
       </c>
     </row>
-    <row r="117" spans="1:42" ht="45" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:42" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A117" s="17" t="s">
         <v>137</v>
       </c>
@@ -22401,7 +22402,7 @@
         <v>1479</v>
       </c>
     </row>
-    <row r="124" spans="1:42" ht="105" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:42" ht="105" hidden="1" x14ac:dyDescent="0.25">
       <c r="A124" s="17" t="s">
         <v>144</v>
       </c>
@@ -22659,7 +22660,7 @@
         <v>1479</v>
       </c>
     </row>
-    <row r="126" spans="1:42" ht="60" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:42" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A126" s="17" t="s">
         <v>146</v>
       </c>
@@ -23676,7 +23677,7 @@
         <v>1479</v>
       </c>
     </row>
-    <row r="134" spans="1:42" ht="30" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:42" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A134" s="17" t="s">
         <v>154</v>
       </c>
@@ -23806,7 +23807,7 @@
         <v>1479</v>
       </c>
     </row>
-    <row r="135" spans="1:42" ht="45" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:42" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A135" s="17" t="s">
         <v>155</v>
       </c>
@@ -24064,7 +24065,7 @@
         <v>1479</v>
       </c>
     </row>
-    <row r="137" spans="1:42" ht="45" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:42" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A137" s="17" t="s">
         <v>157</v>
       </c>
@@ -24322,7 +24323,7 @@
         <v>1479</v>
       </c>
     </row>
-    <row r="139" spans="1:42" ht="210" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:42" ht="210" hidden="1" x14ac:dyDescent="0.25">
       <c r="A139" s="17" t="s">
         <v>159</v>
       </c>
@@ -25220,7 +25221,7 @@
         <v>1479</v>
       </c>
     </row>
-    <row r="146" spans="1:42" ht="90" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:42" ht="90" hidden="1" x14ac:dyDescent="0.25">
       <c r="A146" s="17" t="s">
         <v>166</v>
       </c>
@@ -25348,7 +25349,7 @@
         <v>1479</v>
       </c>
     </row>
-    <row r="147" spans="1:42" ht="45" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:42" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A147" s="17" t="s">
         <v>167</v>
       </c>
@@ -25862,7 +25863,7 @@
         <v>1479</v>
       </c>
     </row>
-    <row r="151" spans="1:42" ht="390" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:42" ht="390" hidden="1" x14ac:dyDescent="0.25">
       <c r="A151" s="17" t="s">
         <v>171</v>
       </c>
@@ -25990,7 +25991,7 @@
         <v>1479</v>
       </c>
     </row>
-    <row r="152" spans="1:42" ht="90" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:42" ht="90" hidden="1" x14ac:dyDescent="0.25">
       <c r="A152" s="17" t="s">
         <v>172</v>
       </c>
@@ -26632,7 +26633,7 @@
         <v>1479</v>
       </c>
     </row>
-    <row r="157" spans="1:42" ht="60" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:42" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A157" s="17" t="s">
         <v>177</v>
       </c>
@@ -26760,7 +26761,7 @@
         <v>1479</v>
       </c>
     </row>
-    <row r="158" spans="1:42" ht="75" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:42" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A158" s="17" t="s">
         <v>178</v>
       </c>
@@ -27920,7 +27921,7 @@
         <v>1479</v>
       </c>
     </row>
-    <row r="167" spans="1:42" ht="90" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:42" ht="90" hidden="1" x14ac:dyDescent="0.25">
       <c r="A167" s="17" t="s">
         <v>187</v>
       </c>
@@ -28305,7 +28306,7 @@
         <v>1479</v>
       </c>
     </row>
-    <row r="170" spans="1:42" ht="45" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:42" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A170" s="17" t="s">
         <v>190</v>
       </c>
@@ -28819,7 +28820,7 @@
         <v>1479</v>
       </c>
     </row>
-    <row r="174" spans="1:42" ht="45" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:42" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A174" s="17" t="s">
         <v>194</v>
       </c>
@@ -29067,7 +29068,7 @@
         <v>1479</v>
       </c>
     </row>
-    <row r="176" spans="1:42" ht="60" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:42" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A176" s="17" t="s">
         <v>196</v>
       </c>
@@ -29195,7 +29196,7 @@
         <v>1479</v>
       </c>
     </row>
-    <row r="177" spans="1:42" ht="60" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:42" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A177" s="17" t="s">
         <v>197</v>
       </c>
@@ -29323,7 +29324,7 @@
         <v>1479</v>
       </c>
     </row>
-    <row r="178" spans="1:42" ht="60" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:42" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A178" s="17" t="s">
         <v>198</v>
       </c>
@@ -29451,7 +29452,7 @@
         <v>1479</v>
       </c>
     </row>
-    <row r="179" spans="1:42" ht="60" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:42" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A179" s="17" t="s">
         <v>199</v>
       </c>
@@ -29579,7 +29580,7 @@
         <v>1479</v>
       </c>
     </row>
-    <row r="180" spans="1:42" ht="60" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:42" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A180" s="17" t="s">
         <v>200</v>
       </c>
@@ -29829,7 +29830,7 @@
         <v>1479</v>
       </c>
     </row>
-    <row r="182" spans="1:42" ht="60" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:42" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A182" s="17" t="s">
         <v>202</v>
       </c>
@@ -29957,7 +29958,7 @@
         <v>1479</v>
       </c>
     </row>
-    <row r="183" spans="1:42" ht="60" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:42" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A183" s="17" t="s">
         <v>203</v>
       </c>
@@ -30085,7 +30086,7 @@
         <v>1479</v>
       </c>
     </row>
-    <row r="184" spans="1:42" ht="60" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:42" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A184" s="17" t="s">
         <v>204</v>
       </c>
@@ -30469,7 +30470,7 @@
         <v>1479</v>
       </c>
     </row>
-    <row r="187" spans="1:42" ht="60" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:42" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A187" s="17" t="s">
         <v>207</v>
       </c>
@@ -30597,7 +30598,7 @@
         <v>1479</v>
       </c>
     </row>
-    <row r="188" spans="1:42" ht="60" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:42" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A188" s="17" t="s">
         <v>208</v>
       </c>
@@ -30713,7 +30714,7 @@
       </c>
       <c r="AP188" s="19"/>
     </row>
-    <row r="189" spans="1:42" ht="60" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:42" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A189" s="17" t="s">
         <v>209</v>
       </c>
@@ -30841,7 +30842,7 @@
         <v>1479</v>
       </c>
     </row>
-    <row r="190" spans="1:42" ht="60" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:42" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A190" s="17" t="s">
         <v>210</v>
       </c>
@@ -30969,7 +30970,7 @@
         <v>1479</v>
       </c>
     </row>
-    <row r="191" spans="1:42" ht="60" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:42" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A191" s="17" t="s">
         <v>211</v>
       </c>
@@ -31097,7 +31098,7 @@
         <v>1479</v>
       </c>
     </row>
-    <row r="192" spans="1:42" ht="60" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:42" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A192" s="17" t="s">
         <v>212</v>
       </c>
@@ -31225,7 +31226,7 @@
         <v>1479</v>
       </c>
     </row>
-    <row r="193" spans="1:42" ht="60" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:42" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A193" s="17" t="s">
         <v>213</v>
       </c>
@@ -31353,7 +31354,7 @@
         <v>1479</v>
       </c>
     </row>
-    <row r="194" spans="1:42" ht="45" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:42" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A194" s="17" t="s">
         <v>214</v>
       </c>
@@ -31481,7 +31482,7 @@
         <v>1479</v>
       </c>
     </row>
-    <row r="195" spans="1:42" ht="60" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:42" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A195" s="17" t="s">
         <v>215</v>
       </c>
@@ -31739,7 +31740,7 @@
         <v>1479</v>
       </c>
     </row>
-    <row r="197" spans="1:42" ht="60" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:42" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A197" s="17" t="s">
         <v>217</v>
       </c>
@@ -31995,7 +31996,7 @@
         <v>1479</v>
       </c>
     </row>
-    <row r="199" spans="1:42" ht="60" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:42" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A199" s="17" t="s">
         <v>219</v>
       </c>
@@ -32251,7 +32252,7 @@
         <v>1479</v>
       </c>
     </row>
-    <row r="201" spans="1:42" ht="60" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:42" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A201" s="17" t="s">
         <v>221</v>
       </c>
@@ -32379,7 +32380,7 @@
         <v>1479</v>
       </c>
     </row>
-    <row r="202" spans="1:42" ht="60" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:42" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A202" s="17" t="s">
         <v>222</v>
       </c>
@@ -32893,7 +32894,7 @@
         <v>1479</v>
       </c>
     </row>
-    <row r="206" spans="1:42" ht="45" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:42" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A206" s="17" t="s">
         <v>226</v>
       </c>
@@ -33021,7 +33022,7 @@
         <v>1479</v>
       </c>
     </row>
-    <row r="207" spans="1:42" ht="90" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:42" ht="90" hidden="1" x14ac:dyDescent="0.25">
       <c r="A207" s="5" t="s">
         <v>227</v>
       </c>
@@ -33148,7 +33149,7 @@
         <v>1479</v>
       </c>
     </row>
-    <row r="208" spans="1:42" ht="90" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:42" ht="90" hidden="1" x14ac:dyDescent="0.25">
       <c r="A208" s="5" t="s">
         <v>228</v>
       </c>
@@ -33276,7 +33277,7 @@
         <v>1479</v>
       </c>
     </row>
-    <row r="209" spans="1:42" ht="90" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:42" ht="90" hidden="1" x14ac:dyDescent="0.25">
       <c r="A209" s="5" t="s">
         <v>229</v>
       </c>
@@ -33404,7 +33405,7 @@
         <v>1479</v>
       </c>
     </row>
-    <row r="210" spans="1:42" ht="90" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:42" ht="90" hidden="1" x14ac:dyDescent="0.25">
       <c r="A210" s="5" t="s">
         <v>230</v>
       </c>
@@ -33532,7 +33533,7 @@
         <v>1479</v>
       </c>
     </row>
-    <row r="211" spans="1:42" ht="90" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:42" ht="90" hidden="1" x14ac:dyDescent="0.25">
       <c r="A211" s="5" t="s">
         <v>231</v>
       </c>
@@ -33660,7 +33661,7 @@
         <v>1479</v>
       </c>
     </row>
-    <row r="212" spans="1:42" ht="90" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:42" ht="90" hidden="1" x14ac:dyDescent="0.25">
       <c r="A212" s="5" t="s">
         <v>232</v>
       </c>
@@ -33788,7 +33789,7 @@
         <v>1479</v>
       </c>
     </row>
-    <row r="213" spans="1:42" ht="90" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:42" ht="90" hidden="1" x14ac:dyDescent="0.25">
       <c r="A213" s="5" t="s">
         <v>233</v>
       </c>
@@ -33916,7 +33917,7 @@
         <v>1479</v>
       </c>
     </row>
-    <row r="214" spans="1:42" ht="90" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:42" ht="90" hidden="1" x14ac:dyDescent="0.25">
       <c r="A214" s="5" t="s">
         <v>234</v>
       </c>
@@ -34044,7 +34045,7 @@
         <v>1479</v>
       </c>
     </row>
-    <row r="215" spans="1:42" ht="30" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:42" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A215" s="5" t="s">
         <v>235</v>
       </c>
@@ -34557,7 +34558,7 @@
         <v>1479</v>
       </c>
     </row>
-    <row r="219" spans="1:42" ht="30" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:42" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A219" s="5" t="s">
         <v>239</v>
       </c>
@@ -34685,7 +34686,7 @@
         <v>1479</v>
       </c>
     </row>
-    <row r="220" spans="1:42" ht="30" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:42" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A220" s="5" t="s">
         <v>240</v>
       </c>
@@ -35955,7 +35956,7 @@
         <v>1479</v>
       </c>
     </row>
-    <row r="230" spans="1:42" ht="30" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:42" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A230" s="5" t="s">
         <v>250</v>
       </c>
@@ -36085,7 +36086,7 @@
         <v>1479</v>
       </c>
     </row>
-    <row r="231" spans="1:42" ht="45" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:42" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A231" s="5" t="s">
         <v>251</v>
       </c>
@@ -36214,7 +36215,7 @@
         <v>1479</v>
       </c>
     </row>
-    <row r="232" spans="1:42" ht="30" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:42" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A232" s="5" t="s">
         <v>252</v>
       </c>
@@ -36343,7 +36344,7 @@
         <v>1479</v>
       </c>
     </row>
-    <row r="233" spans="1:42" ht="30" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:42" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A233" s="5" t="s">
         <v>253</v>
       </c>
@@ -36598,7 +36599,7 @@
         <v>1479</v>
       </c>
     </row>
-    <row r="235" spans="1:42" ht="60" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:42" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A235" s="5" t="s">
         <v>254</v>
       </c>
@@ -36725,7 +36726,7 @@
         <v>1479</v>
       </c>
     </row>
-    <row r="236" spans="1:42" ht="90" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:42" ht="90" hidden="1" x14ac:dyDescent="0.25">
       <c r="A236" s="5" t="s">
         <v>255</v>
       </c>
@@ -36848,7 +36849,7 @@
         <v>1479</v>
       </c>
     </row>
-    <row r="237" spans="1:42" ht="30" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:42" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A237" s="5" t="s">
         <v>256</v>
       </c>
@@ -36978,7 +36979,7 @@
         <v>1479</v>
       </c>
     </row>
-    <row r="238" spans="1:42" ht="30" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:42" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A238" s="5" t="s">
         <v>257</v>
       </c>
@@ -37108,7 +37109,7 @@
         <v>1479</v>
       </c>
     </row>
-    <row r="239" spans="1:42" ht="30" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:42" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A239" s="5" t="s">
         <v>258</v>
       </c>
@@ -37238,7 +37239,7 @@
         <v>1479</v>
       </c>
     </row>
-    <row r="240" spans="1:42" ht="75" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:42" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A240" s="5" t="s">
         <v>259</v>
       </c>
@@ -37368,7 +37369,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="241" spans="1:42" ht="30" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:42" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A241" s="5" t="s">
         <v>260</v>
       </c>
@@ -37495,7 +37496,7 @@
         <v>1479</v>
       </c>
     </row>
-    <row r="242" spans="1:42" ht="45" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:42" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A242" s="5" t="s">
         <v>261</v>
       </c>
@@ -37625,7 +37626,7 @@
         <v>1479</v>
       </c>
     </row>
-    <row r="243" spans="1:42" ht="45" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:42" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A243" s="5" t="s">
         <v>262</v>
       </c>
@@ -37755,7 +37756,7 @@
         <v>1479</v>
       </c>
     </row>
-    <row r="244" spans="1:42" ht="30" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:42" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A244" s="5" t="s">
         <v>263</v>
       </c>
@@ -37882,7 +37883,7 @@
         <v>1479</v>
       </c>
     </row>
-    <row r="245" spans="1:42" ht="30" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:42" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A245" s="5" t="s">
         <v>264</v>
       </c>
@@ -38012,7 +38013,7 @@
         <v>1479</v>
       </c>
     </row>
-    <row r="246" spans="1:42" ht="45" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:42" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A246" s="5" t="s">
         <v>265</v>
       </c>
@@ -38142,7 +38143,7 @@
         <v>1479</v>
       </c>
     </row>
-    <row r="247" spans="1:42" ht="30" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:42" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A247" s="5" t="s">
         <v>266</v>
       </c>
@@ -38272,7 +38273,7 @@
         <v>1479</v>
       </c>
     </row>
-    <row r="248" spans="1:42" ht="30" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:42" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A248" s="5" t="s">
         <v>267</v>
       </c>
@@ -38403,7 +38404,7 @@
         <v>1479</v>
       </c>
     </row>
-    <row r="249" spans="1:42" ht="30" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:42" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A249" s="5" t="s">
         <v>268</v>
       </c>
@@ -38660,7 +38661,7 @@
         <v>1479</v>
       </c>
     </row>
-    <row r="251" spans="1:42" ht="30" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:42" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A251" s="5" t="s">
         <v>269</v>
       </c>
@@ -38790,7 +38791,7 @@
         <v>1479</v>
       </c>
     </row>
-    <row r="252" spans="1:42" ht="30" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:42" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A252" s="5" t="s">
         <v>270</v>
       </c>
@@ -38920,7 +38921,7 @@
         <v>1479</v>
       </c>
     </row>
-    <row r="253" spans="1:42" ht="30" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:42" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A253" s="5" t="s">
         <v>271</v>
       </c>
@@ -39050,7 +39051,7 @@
         <v>1479</v>
       </c>
     </row>
-    <row r="254" spans="1:42" ht="45" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:42" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A254" s="5" t="s">
         <v>272</v>
       </c>
@@ -39180,7 +39181,7 @@
         <v>1479</v>
       </c>
     </row>
-    <row r="255" spans="1:42" ht="45" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:42" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A255" s="5" t="s">
         <v>273</v>
       </c>
@@ -39308,7 +39309,7 @@
         <v>1479</v>
       </c>
     </row>
-    <row r="256" spans="1:42" ht="30" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:42" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A256" s="5" t="s">
         <v>274</v>
       </c>
@@ -39438,7 +39439,7 @@
         <v>1479</v>
       </c>
     </row>
-    <row r="257" spans="1:42" ht="60" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:42" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A257" s="5" t="s">
         <v>275</v>
       </c>
@@ -39568,7 +39569,7 @@
         <v>1479</v>
       </c>
     </row>
-    <row r="258" spans="1:42" ht="30" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:42" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A258" s="5" t="s">
         <v>276</v>
       </c>
@@ -39698,7 +39699,7 @@
         <v>1479</v>
       </c>
     </row>
-    <row r="259" spans="1:42" ht="30" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:42" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A259" s="5" t="s">
         <v>277</v>
       </c>
@@ -39828,7 +39829,7 @@
         <v>1479</v>
       </c>
     </row>
-    <row r="260" spans="1:42" ht="30" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:42" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A260" s="5" t="s">
         <v>278</v>
       </c>
@@ -39958,7 +39959,7 @@
         <v>1600</v>
       </c>
     </row>
-    <row r="261" spans="1:42" ht="30" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:42" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A261" s="5" t="s">
         <v>279</v>
       </c>
@@ -40088,7 +40089,7 @@
         <v>1479</v>
       </c>
     </row>
-    <row r="262" spans="1:42" ht="30" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:42" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A262" s="5" t="s">
         <v>280</v>
       </c>
@@ -40217,7 +40218,7 @@
         <v>1479</v>
       </c>
     </row>
-    <row r="263" spans="1:42" ht="30" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:42" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A263" s="5" t="s">
         <v>281</v>
       </c>
@@ -40347,7 +40348,7 @@
         <v>1479</v>
       </c>
     </row>
-    <row r="264" spans="1:42" ht="30" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:42" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A264" s="5" t="s">
         <v>282</v>
       </c>
@@ -40477,7 +40478,7 @@
         <v>1479</v>
       </c>
     </row>
-    <row r="265" spans="1:42" ht="30" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:42" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A265" s="5" t="s">
         <v>283</v>
       </c>
@@ -40608,7 +40609,7 @@
         <v>1479</v>
       </c>
     </row>
-    <row r="266" spans="1:42" ht="30" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:42" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A266" s="5" t="s">
         <v>284</v>
       </c>
@@ -40738,7 +40739,7 @@
         <v>1479</v>
       </c>
     </row>
-    <row r="267" spans="1:42" ht="30" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:42" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A267" s="5" t="s">
         <v>285</v>
       </c>
@@ -40868,7 +40869,7 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="268" spans="1:42" ht="60" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:42" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A268" s="5" t="s">
         <v>286</v>
       </c>
@@ -40997,7 +40998,7 @@
         <v>1479</v>
       </c>
     </row>
-    <row r="269" spans="1:42" ht="30" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:42" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A269" s="5" t="s">
         <v>287</v>
       </c>
@@ -41127,7 +41128,7 @@
         <v>1479</v>
       </c>
     </row>
-    <row r="270" spans="1:42" ht="45" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:42" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A270" s="5" t="s">
         <v>288</v>
       </c>
@@ -41257,7 +41258,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="271" spans="1:42" ht="30" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:42" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A271" s="5" t="s">
         <v>289</v>
       </c>
@@ -41386,7 +41387,7 @@
         <v>1479</v>
       </c>
     </row>
-    <row r="272" spans="1:42" ht="30" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:42" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A272" s="5" t="s">
         <v>290</v>
       </c>
@@ -41516,7 +41517,7 @@
         <v>1479</v>
       </c>
     </row>
-    <row r="273" spans="1:42" ht="75" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:42" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A273" s="5" t="s">
         <v>291</v>
       </c>
@@ -41645,7 +41646,7 @@
         <v>1479</v>
       </c>
     </row>
-    <row r="274" spans="1:42" ht="30" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:42" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A274" s="5" t="s">
         <v>292</v>
       </c>
@@ -41903,7 +41904,7 @@
         <v>1479</v>
       </c>
     </row>
-    <row r="276" spans="1:42" ht="30" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:42" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A276" s="5" t="s">
         <v>1531</v>
       </c>
@@ -42033,7 +42034,7 @@
         <v>1479</v>
       </c>
     </row>
-    <row r="277" spans="1:42" ht="30" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:42" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A277" s="5" t="s">
         <v>293</v>
       </c>
@@ -42164,7 +42165,7 @@
         <v>1479</v>
       </c>
     </row>
-    <row r="278" spans="1:42" ht="60" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:42" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A278" s="5" t="s">
         <v>294</v>
       </c>
@@ -42293,7 +42294,7 @@
         <v>1479</v>
       </c>
     </row>
-    <row r="279" spans="1:42" ht="45" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:42" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A279" s="5" t="s">
         <v>295</v>
       </c>
@@ -42423,7 +42424,7 @@
         <v>1479</v>
       </c>
     </row>
-    <row r="280" spans="1:42" ht="60" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:42" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A280" s="5" t="s">
         <v>296</v>
       </c>
@@ -42552,7 +42553,7 @@
         <v>1479</v>
       </c>
     </row>
-    <row r="281" spans="1:42" ht="75" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:42" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A281" s="5" t="s">
         <v>297</v>
       </c>
@@ -42681,7 +42682,7 @@
         <v>1479</v>
       </c>
     </row>
-    <row r="282" spans="1:42" ht="90" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:42" ht="90" hidden="1" x14ac:dyDescent="0.25">
       <c r="A282" s="5" t="s">
         <v>298</v>
       </c>
@@ -42811,7 +42812,7 @@
         <v>1479</v>
       </c>
     </row>
-    <row r="283" spans="1:42" ht="45" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:42" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A283" s="5" t="s">
         <v>299</v>
       </c>
@@ -42940,7 +42941,7 @@
         <v>1479</v>
       </c>
     </row>
-    <row r="284" spans="1:42" ht="30" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:42" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A284" s="5" t="s">
         <v>300</v>
       </c>
@@ -43070,7 +43071,7 @@
         <v>1479</v>
       </c>
     </row>
-    <row r="285" spans="1:42" ht="75" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:42" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A285" s="5" t="s">
         <v>301</v>
       </c>
@@ -43199,7 +43200,7 @@
         <v>1479</v>
       </c>
     </row>
-    <row r="286" spans="1:42" ht="75" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:42" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A286" s="5" t="s">
         <v>302</v>
       </c>
@@ -43328,7 +43329,7 @@
         <v>1479</v>
       </c>
     </row>
-    <row r="287" spans="1:42" ht="60" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:42" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A287" s="5" t="s">
         <v>303</v>
       </c>
@@ -43459,7 +43460,7 @@
         <v>1479</v>
       </c>
     </row>
-    <row r="288" spans="1:42" ht="30" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:42" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A288" s="5" t="s">
         <v>304</v>
       </c>
@@ -43588,7 +43589,7 @@
         <v>1479</v>
       </c>
     </row>
-    <row r="289" spans="1:42" ht="60" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:42" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A289" s="5" t="s">
         <v>305</v>
       </c>
@@ -43717,7 +43718,7 @@
         <v>1479</v>
       </c>
     </row>
-    <row r="290" spans="1:42" ht="30" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:42" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A290" s="5" t="s">
         <v>306</v>
       </c>
@@ -43975,7 +43976,7 @@
         <v>1479</v>
       </c>
     </row>
-    <row r="292" spans="1:42" ht="90" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:42" ht="90" hidden="1" x14ac:dyDescent="0.25">
       <c r="A292" s="5" t="s">
         <v>308</v>
       </c>
@@ -44104,7 +44105,7 @@
         <v>1479</v>
       </c>
     </row>
-    <row r="293" spans="1:42" ht="30" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:42" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A293" s="5" t="s">
         <v>309</v>
       </c>
@@ -44233,7 +44234,7 @@
         <v>1479</v>
       </c>
     </row>
-    <row r="294" spans="1:42" ht="75" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:42" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A294" s="5" t="s">
         <v>310</v>
       </c>
@@ -44362,7 +44363,7 @@
         <v>1479</v>
       </c>
     </row>
-    <row r="295" spans="1:42" ht="45" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:42" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A295" s="5" t="s">
         <v>311</v>
       </c>
@@ -44491,7 +44492,7 @@
         <v>1479</v>
       </c>
     </row>
-    <row r="296" spans="1:42" ht="45" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:42" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A296" s="5" t="s">
         <v>312</v>
       </c>
@@ -44620,7 +44621,7 @@
         <v>1479</v>
       </c>
     </row>
-    <row r="297" spans="1:42" ht="75" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:42" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A297" s="5" t="s">
         <v>313</v>
       </c>
@@ -44750,7 +44751,7 @@
         <v>1479</v>
       </c>
     </row>
-    <row r="298" spans="1:42" ht="75" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:42" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A298" s="5" t="s">
         <v>314</v>
       </c>
@@ -44879,7 +44880,7 @@
         <v>1479</v>
       </c>
     </row>
-    <row r="299" spans="1:42" ht="30" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:42" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A299" s="5" t="s">
         <v>315</v>
       </c>
@@ -45137,7 +45138,7 @@
         <v>1479</v>
       </c>
     </row>
-    <row r="301" spans="1:42" ht="45" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:42" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A301" s="5" t="s">
         <v>317</v>
       </c>
@@ -45395,7 +45396,7 @@
         <v>1479</v>
       </c>
     </row>
-    <row r="303" spans="1:42" ht="90" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:42" ht="90" hidden="1" x14ac:dyDescent="0.25">
       <c r="A303" s="5" t="s">
         <v>318</v>
       </c>
@@ -45525,7 +45526,7 @@
         <v>1479</v>
       </c>
     </row>
-    <row r="304" spans="1:42" ht="90" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:42" ht="90" hidden="1" x14ac:dyDescent="0.25">
       <c r="A304" s="5" t="s">
         <v>319</v>
       </c>
@@ -45655,7 +45656,7 @@
         <v>1479</v>
       </c>
     </row>
-    <row r="305" spans="1:42" ht="90" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:42" ht="90" hidden="1" x14ac:dyDescent="0.25">
       <c r="A305" s="5" t="s">
         <v>320</v>
       </c>
@@ -45785,7 +45786,7 @@
         <v>1479</v>
       </c>
     </row>
-    <row r="306" spans="1:42" ht="90" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:42" ht="90" hidden="1" x14ac:dyDescent="0.25">
       <c r="A306" s="5" t="s">
         <v>321</v>
       </c>
@@ -45915,7 +45916,7 @@
         <v>1479</v>
       </c>
     </row>
-    <row r="307" spans="1:42" ht="30" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:42" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A307" s="5" t="s">
         <v>322</v>
       </c>
@@ -46302,7 +46303,7 @@
         <v>1479</v>
       </c>
     </row>
-    <row r="310" spans="1:42" ht="90" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:42" ht="90" hidden="1" x14ac:dyDescent="0.25">
       <c r="A310" s="5" t="s">
         <v>325</v>
       </c>
@@ -46432,7 +46433,7 @@
         <v>1479</v>
       </c>
     </row>
-    <row r="311" spans="1:42" ht="45" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:42" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A311" s="5" t="s">
         <v>326</v>
       </c>
@@ -47207,7 +47208,7 @@
         <v>1479</v>
       </c>
     </row>
-    <row r="317" spans="1:42" ht="30" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:42" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A317" s="5" t="s">
         <v>332</v>
       </c>
@@ -48497,7 +48498,7 @@
         <v>1479</v>
       </c>
     </row>
-    <row r="327" spans="1:42" ht="60" x14ac:dyDescent="0.25">
+    <row r="327" spans="1:42" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A327" s="5" t="s">
         <v>342</v>
       </c>
@@ -48626,7 +48627,7 @@
         <v>1479</v>
       </c>
     </row>
-    <row r="328" spans="1:42" ht="120" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:42" ht="120" hidden="1" x14ac:dyDescent="0.25">
       <c r="A328" s="5" t="s">
         <v>343</v>
       </c>
@@ -48755,7 +48756,7 @@
         <v>1479</v>
       </c>
     </row>
-    <row r="329" spans="1:42" ht="30" x14ac:dyDescent="0.25">
+    <row r="329" spans="1:42" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A329" s="5" t="s">
         <v>344</v>
       </c>
@@ -49659,7 +49660,7 @@
         <v>1479</v>
       </c>
     </row>
-    <row r="336" spans="1:42" ht="45" x14ac:dyDescent="0.25">
+    <row r="336" spans="1:42" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A336" s="5" t="s">
         <v>351</v>
       </c>
@@ -50564,7 +50565,7 @@
         <v>1479</v>
       </c>
     </row>
-    <row r="343" spans="1:42" ht="75" x14ac:dyDescent="0.25">
+    <row r="343" spans="1:42" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A343" s="5" t="s">
         <v>358</v>
       </c>
@@ -50822,7 +50823,7 @@
         <v>1479</v>
       </c>
     </row>
-    <row r="345" spans="1:42" ht="45" x14ac:dyDescent="0.25">
+    <row r="345" spans="1:42" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A345" s="5" t="s">
         <v>360</v>
       </c>
@@ -51210,7 +51211,7 @@
         <v>1479</v>
       </c>
     </row>
-    <row r="348" spans="1:42" ht="30" x14ac:dyDescent="0.25">
+    <row r="348" spans="1:42" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A348" s="5" t="s">
         <v>362</v>
       </c>
@@ -52371,7 +52372,7 @@
         <v>1479</v>
       </c>
     </row>
-    <row r="357" spans="1:42" ht="45" x14ac:dyDescent="0.25">
+    <row r="357" spans="1:42" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A357" s="5" t="s">
         <v>371</v>
       </c>
@@ -52888,7 +52889,7 @@
         <v>1479</v>
       </c>
     </row>
-    <row r="361" spans="1:42" ht="90" x14ac:dyDescent="0.25">
+    <row r="361" spans="1:42" ht="90" hidden="1" x14ac:dyDescent="0.25">
       <c r="A361" s="5" t="s">
         <v>375</v>
       </c>
@@ -53146,7 +53147,7 @@
         <v>1479</v>
       </c>
     </row>
-    <row r="363" spans="1:42" ht="45" x14ac:dyDescent="0.25">
+    <row r="363" spans="1:42" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A363" s="5" t="s">
         <v>377</v>
       </c>
@@ -53405,7 +53406,7 @@
         <v>1479</v>
       </c>
     </row>
-    <row r="365" spans="1:42" ht="30" x14ac:dyDescent="0.25">
+    <row r="365" spans="1:42" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A365" s="5" t="s">
         <v>379</v>
       </c>
@@ -54695,7 +54696,7 @@
         <v>1479</v>
       </c>
     </row>
-    <row r="375" spans="1:42" ht="45" x14ac:dyDescent="0.25">
+    <row r="375" spans="1:42" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A375" s="5" t="s">
         <v>389</v>
       </c>
@@ -55470,7 +55471,7 @@
         <v>1479</v>
       </c>
     </row>
-    <row r="381" spans="1:42" ht="45" x14ac:dyDescent="0.25">
+    <row r="381" spans="1:42" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A381" s="5" t="s">
         <v>395</v>
       </c>
@@ -57390,7 +57391,7 @@
         <v>1479</v>
       </c>
     </row>
-    <row r="396" spans="1:42" ht="45" x14ac:dyDescent="0.25">
+    <row r="396" spans="1:42" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A396" s="5"/>
       <c r="B396" s="6" t="s">
         <v>402</v>
@@ -57655,7 +57656,13 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AP397" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:AP397" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <filterColumn colId="21">
+      <filters>
+        <filter val="Não"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <dataValidations count="3">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K2:K3 V2:V5 K7 V7 K15 V15 K25 V25 X25 K33 V33 X33 K36:K38 V36:V38 X36:X38 K45 V45 X45 K47 V47 X47 K53 V53 X53 K125 V125 X125 K134 K136:K137 V138 X138 K140 V140 X140 K158:K159 V159 X159 K164:K165 V163:V165 X163:X165 K59:K60 V59:V60 X59:X60 K62 V62 X62 K66 V66 X66 V88 X88 V99 X99 V116 X116 V118 X118 V123 X123 V127:V128 X127:X128 V136 X136 K154 V154:V155 X154:X155 K173 V173 X173" xr:uid="{ADB4BF40-33A8-4989-A35D-007296DFD734}">
       <formula1>"Sim, Não"</formula1>

</xml_diff>